<commit_message>
debug(wrapper): Disable infor dict modification to test for memory leak
</commit_message>
<xml_diff>
--- a/Eval_Run_Logs.xlsx
+++ b/Eval_Run_Logs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Github\DeepRL-MsPacman\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CFB506-C759-4268-9E0D-A23A563C38FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D4C6BAD-DD81-4850-A49E-E3A95191803F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{0D67D52D-1513-48BB-A273-B9082DA3F499}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0D67D52D-1513-48BB-A273-B9082DA3F499}"/>
   </bookViews>
   <sheets>
     <sheet name="DQN_Runs" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -197,7 +197,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -537,7 +537,7 @@
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,10 +675,10 @@
         <v>5000</v>
       </c>
       <c r="N2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>